<commit_message>
Update Recipes_in_Orders table to include item_number
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NELSON K. CHAN\Google Drive\My Documents\Oregon State University\CS 340 Intro to Databases\Group 11\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessm\Documents\OSU\CS340 - Databases\CS340_W2020_group11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF880368-7935-4049-94AF-02951048F3AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C569A717-7984-4A11-AEA5-A04893CF6F4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{535123E1-B282-4026-BBB3-142D2E158CD6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{535123E1-B282-4026-BBB3-142D2E158CD6}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>customer_id</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>ingredients</t>
+  </si>
+  <si>
+    <t>item_number</t>
   </si>
 </sst>
 </file>
@@ -568,16 +571,16 @@
   <dimension ref="B1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H2"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.5625" defaultRowHeight="13.15" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="15.5625" style="1"/>
+    <col min="1" max="16384" width="15.59765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="2" spans="2:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
@@ -588,7 +591,7 @@
       <c r="G2" s="7"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="2:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -611,8 +614,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="6" spans="2:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
@@ -623,7 +626,7 @@
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="2:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
@@ -642,8 +645,8 @@
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="9" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="10" spans="2:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="2:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
@@ -653,7 +656,7 @@
       <c r="F10" s="8"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -670,8 +673,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="14" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
@@ -680,7 +683,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>12</v>
       </c>
@@ -697,19 +700,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="18" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>